<commit_message>
adding a code delete Notification
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/API_List (1).xlsx
+++ b/src/test/java/TestData/API_List (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Core_Java\TAXI_BOOKING_RestAssured\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Core_Java\taxi-booking-api-automation\src\test\java\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A140D49C-2DC3-422C-843D-DF42331A5C2B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA9A8EF-0E9E-4008-B999-2C74468E9064}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -797,7 +797,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>

</xml_diff>